<commit_message>
Code has run. Still have bug in socket (guess)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Desktop\DATN_git\Socket_Want_To_Go_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11000D49-8839-41E3-80CE-04878306AD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F574908F-E82B-49E4-812C-57FFD6916375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,10 @@
     <t>Done Server, Client.
 Fix Aggregate function.
 Not debug yet.</t>
+  </si>
+  <si>
+    <t>Code Run.
+Still have bug (guess in socket creating and closing).</t>
   </si>
 </sst>
 </file>
@@ -75,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -94,12 +98,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -138,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,11 +180,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,7 +472,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +490,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -482,25 +501,25 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>45691</v>
+        <v>45718</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>45692</v>
+        <v>45384</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -509,117 +528,131 @@
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>45963.497916666667</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>45993.070138888892</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="C8" s="9"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>45993.765972222223</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="9"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:C4"/>
-    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C5:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Debug socket. Still have 1 bug in 'first client'
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Desktop\DATN_git\Socket_Want_To_Go_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F574908F-E82B-49E4-812C-57FFD6916375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE33E5-BC1B-4A36-9826-8FD36CDB8D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,13 @@
   <si>
     <t>Code Run.
 Still have bug (guess in socket creating and closing).</t>
+  </si>
+  <si>
+    <t>13/2/25 1:25 PM</t>
+  </si>
+  <si>
+    <t>Debug socket.
+Still have bug (when run, every first client will be pending forever)</t>
   </si>
 </sst>
 </file>
@@ -154,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,9 +177,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -472,12 +476,12 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="92.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
@@ -490,7 +494,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -501,7 +505,7 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -510,7 +514,7 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -519,135 +523,140 @@
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>45932.635810185187</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="8">
+        <v>45932.635416666664</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>45963.497916666667</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>45993.070138888892</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="8">
+        <v>45993.570138888892</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>45993.765972222223</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="C9" s="11"/>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="8"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="8"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="8"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="8"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="8"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="8"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="8"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="8"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="8"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="8"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="8"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>